<commit_message>
Homework 8 and associated slides
</commit_message>
<xml_diff>
--- a/Outcome_Mapping.xlsx
+++ b/Outcome_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfdeblasio/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deblasio/Google_Drive/Classes/CS2101.2202/CS2101 (1).CS2202.Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F215A6-BD04-1049-8AA3-32FADAC99736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA71DEB-F601-C645-B7EB-1A4512EFC226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16200" yWindow="5880" windowWidth="27640" windowHeight="16940" xr2:uid="{9E64036C-C5FF-F54A-80AF-497F704BC684}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{9E64036C-C5FF-F54A-80AF-497F704BC684}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes to Questions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
   <si>
     <t>DS 1</t>
   </si>
@@ -153,6 +152,33 @@
   </si>
   <si>
     <t>Homework</t>
+  </si>
+  <si>
+    <t>Long Quiz 2</t>
+  </si>
+  <si>
+    <t>Q1-4</t>
+  </si>
+  <si>
+    <t>Q5-6</t>
+  </si>
+  <si>
+    <t>Long Quiz 3</t>
+  </si>
+  <si>
+    <t>HW4</t>
+  </si>
+  <si>
+    <t>HW5</t>
+  </si>
+  <si>
+    <t>HW6</t>
+  </si>
+  <si>
+    <t>HW7</t>
+  </si>
+  <si>
+    <t>HW8</t>
   </si>
 </sst>
 </file>
@@ -235,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -254,6 +280,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -263,14 +292,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -591,13 +660,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4002F2A3-909B-0246-BCD5-76C89B754559}">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:AH40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="AH32" sqref="AH32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,28 +675,43 @@
     <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" style="7"/>
+    <col min="17" max="17" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="D1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -673,17 +757,40 @@
       <c r="P2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" t="s">
         <v>35</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AB2" t="s">
         <v>36</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AC2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="AD2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -691,59 +798,82 @@
       <c r="C3" s="1"/>
       <c r="D3" s="5"/>
       <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U3" s="6"/>
+      <c r="Z3" s="6"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4">
-        <f>SUM(D4:P4)</f>
+        <f>SUM(D4:U4)</f>
         <v>0</v>
       </c>
       <c r="C4" s="4">
-        <f>SUM(Q5:S5)</f>
-        <v>1</v>
+        <f>SUM(AA4:AH4)</f>
+        <v>3</v>
       </c>
       <c r="D4" s="5"/>
       <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4">
-        <f>SUM(D5:P5)</f>
-        <v>1</v>
+        <f>SUM(D5:U5)</f>
+        <v>5</v>
       </c>
       <c r="C5" s="4">
-        <f>SUM(Q6:S6)</f>
-        <v>0</v>
+        <f>SUM(AA5:AH5)</f>
+        <v>2</v>
       </c>
       <c r="D5" s="5"/>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="P5" s="6"/>
-      <c r="S5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="Q5" s="7">
+        <v>4</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4">
-        <f>SUM(D6:P6)</f>
+        <f>SUM(D6:U6)</f>
         <v>0</v>
       </c>
       <c r="C6" s="4">
-        <f>SUM(Q7:S7)</f>
+        <f>SUM(AA6:AH6)</f>
         <v>0</v>
       </c>
       <c r="D6" s="5"/>
       <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U6" s="6"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -751,17 +881,19 @@
       <c r="C7" s="1"/>
       <c r="D7" s="5"/>
       <c r="P7" s="6"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U7" s="6"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4">
-        <f>SUM(D8:P8)</f>
+        <f>SUM(D8:U8)</f>
         <v>1</v>
       </c>
       <c r="C8" s="4">
-        <f>SUM(Q9:S9)</f>
+        <f>SUM(AA8:AH8)</f>
         <v>2</v>
       </c>
       <c r="D8" s="5"/>
@@ -769,21 +901,26 @@
         <v>1</v>
       </c>
       <c r="P8" s="6"/>
-      <c r="S8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4">
-        <f>SUM(D9:P9)</f>
+        <f>SUM(D9:U9)</f>
         <v>9</v>
       </c>
       <c r="C9" s="4">
-        <f>SUM(Q10:S10)</f>
-        <v>0</v>
+        <f>SUM(AA9:AH9)</f>
+        <v>5</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
@@ -812,14 +949,25 @@
       <c r="P9" s="6">
         <v>1</v>
       </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -827,59 +975,73 @@
       <c r="C10" s="1"/>
       <c r="D10" s="5"/>
       <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="U10" s="6"/>
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="4">
-        <f>SUM(D11:P11)</f>
+        <f>SUM(D11:U11)</f>
         <v>1</v>
       </c>
       <c r="C11" s="4">
-        <f>SUM(Q12:S12)</f>
-        <v>0</v>
+        <f>SUM(AA11:AH11)</f>
+        <v>1</v>
       </c>
       <c r="D11" s="5"/>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="P11" s="6"/>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="4">
-        <f>SUM(D12:P12)</f>
-        <v>0</v>
+        <f>SUM(D12:U12)</f>
+        <v>2</v>
       </c>
       <c r="C12" s="4">
-        <f>SUM(Q13:S13)</f>
-        <v>0</v>
+        <f>SUM(AA12:AH12)</f>
+        <v>1</v>
       </c>
       <c r="D12" s="5"/>
       <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="U12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AE12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="4">
-        <f>SUM(D13:P13)</f>
+        <f>SUM(D13:U13)</f>
         <v>0</v>
       </c>
       <c r="C13" s="4">
-        <f>SUM(Q14:S14)</f>
+        <f>SUM(AA13:AH13)</f>
         <v>0</v>
       </c>
       <c r="D13" s="5"/>
       <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U13" s="6"/>
+      <c r="Z13" s="6"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -896,11 +1058,26 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="11"/>
-      <c r="Q14" s="8"/>
+      <c r="Q14" s="10"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14" s="8"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -943,17 +1120,62 @@
         <v>33</v>
       </c>
       <c r="P15" s="6"/>
-      <c r="Q15" t="s">
+      <c r="Q15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S15" t="s">
+        <v>3</v>
+      </c>
+      <c r="T15" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" t="s">
+        <v>2</v>
+      </c>
+      <c r="X15" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA15" t="s">
         <v>35</v>
       </c>
-      <c r="R15" t="s">
+      <c r="AB15" t="s">
         <v>36</v>
       </c>
-      <c r="S15" t="s">
+      <c r="AC15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="AD15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -961,69 +1183,98 @@
       <c r="C16" s="1"/>
       <c r="D16" s="5"/>
       <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="U16" s="6"/>
+      <c r="V16" s="7"/>
+      <c r="Z16" s="6"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="4">
-        <f>SUM(D17:P17)</f>
+        <f>SUM(D17:Z17)</f>
         <v>0</v>
       </c>
       <c r="C17" s="4">
-        <f>SUM(Q18:S18)</f>
-        <v>0</v>
+        <f>SUM(AA17:AH17)</f>
+        <v>1</v>
       </c>
       <c r="D17" s="5"/>
       <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U17" s="6"/>
+      <c r="V17" s="7"/>
+      <c r="Z17" s="6"/>
+      <c r="AH17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="4">
-        <f>SUM(D18:P18)</f>
-        <v>0</v>
+        <f>SUM(D18:Z18)</f>
+        <v>1</v>
       </c>
       <c r="C18" s="4">
-        <f>SUM(Q19:S19)</f>
-        <v>1</v>
+        <f>SUM(AA18:AH18)</f>
+        <v>2</v>
       </c>
       <c r="D18" s="5"/>
       <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U18" s="6"/>
+      <c r="V18" s="7"/>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="6"/>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AG18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="4">
-        <f>SUM(D19:P19)</f>
-        <v>1</v>
+        <f>SUM(D19:Z19)</f>
+        <v>2</v>
       </c>
       <c r="C19" s="4">
-        <f>SUM(Q20:S20)</f>
-        <v>1</v>
+        <f>SUM(AA19:AH19)</f>
+        <v>2</v>
       </c>
       <c r="D19" s="5"/>
       <c r="J19">
         <v>1</v>
       </c>
       <c r="P19" s="6"/>
-      <c r="R19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U19" s="6">
+        <v>1</v>
+      </c>
+      <c r="V19" s="7"/>
+      <c r="Z19" s="6"/>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AG19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="4">
-        <f>SUM(D20:P20)</f>
+        <f>SUM(D20:Z20)</f>
         <v>2</v>
       </c>
       <c r="C20" s="4">
-        <f>SUM(Q21:S21)</f>
-        <v>0</v>
+        <f>SUM(AA20:AH20)</f>
+        <v>1</v>
       </c>
       <c r="D20" s="5"/>
       <c r="H20">
@@ -1033,11 +1284,14 @@
         <v>1</v>
       </c>
       <c r="P20" s="6"/>
-      <c r="S20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U20" s="6"/>
+      <c r="V20" s="7"/>
+      <c r="Z20" s="6"/>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1045,33 +1299,45 @@
       <c r="C21" s="1"/>
       <c r="D21" s="5"/>
       <c r="P21" s="6"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U21" s="6"/>
+      <c r="V21" s="7"/>
+      <c r="Z21" s="6"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="4">
-        <f>SUM(D22:P22)</f>
-        <v>0</v>
+        <f>SUM(D22:Z22)</f>
+        <v>1</v>
       </c>
       <c r="C22" s="4">
-        <f>SUM(Q23:S23)</f>
-        <v>0</v>
+        <f>SUM(AA22:AH22)</f>
+        <v>1</v>
       </c>
       <c r="D22" s="5"/>
       <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q22" s="7">
+        <v>1</v>
+      </c>
+      <c r="U22" s="6"/>
+      <c r="V22" s="7"/>
+      <c r="Z22" s="6"/>
+      <c r="AE22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="4">
-        <f>SUM(D23:P23)</f>
-        <v>2</v>
+        <f>SUM(D23:Z23)</f>
+        <v>6</v>
       </c>
       <c r="C23" s="4">
-        <f>SUM(Q24:S24)</f>
-        <v>0</v>
+        <f>SUM(AA23:AH23)</f>
+        <v>2</v>
       </c>
       <c r="D23" s="5"/>
       <c r="F23">
@@ -1081,18 +1347,39 @@
         <v>1</v>
       </c>
       <c r="P23" s="6"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q23" s="7">
+        <v>1</v>
+      </c>
+      <c r="R23" s="7">
+        <v>1</v>
+      </c>
+      <c r="S23" s="7">
+        <v>1</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1</v>
+      </c>
+      <c r="U23" s="6"/>
+      <c r="V23" s="7"/>
+      <c r="Z23" s="6"/>
+      <c r="AD23">
+        <v>1</v>
+      </c>
+      <c r="AE23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="4">
-        <f>SUM(D24:P24)</f>
+        <f>SUM(D24:Z24)</f>
         <v>2</v>
       </c>
       <c r="C24" s="4">
-        <f>SUM(Q25:S25)</f>
-        <v>0</v>
+        <f>SUM(AA24:AH24)</f>
+        <v>2</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24">
@@ -1102,38 +1389,78 @@
         <v>1</v>
       </c>
       <c r="P24" s="6"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U24" s="6"/>
+      <c r="V24" s="7"/>
+      <c r="Z24" s="6"/>
+      <c r="AD24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="4">
-        <f>SUM(D25:P25)</f>
-        <v>0</v>
+        <f>SUM(D25:Z25)</f>
+        <v>4</v>
       </c>
       <c r="C25" s="4">
-        <f>SUM(Q26:S26)</f>
-        <v>0</v>
+        <f>SUM(AA25:AH25)</f>
+        <v>2</v>
       </c>
       <c r="D25" s="5"/>
       <c r="P25" s="6"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U25" s="6"/>
+      <c r="V25" s="7">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF25">
+        <v>1</v>
+      </c>
+      <c r="AG25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="4">
-        <f>SUM(D26:P26)</f>
-        <v>0</v>
+        <f>SUM(D26:Z26)</f>
+        <v>1</v>
       </c>
       <c r="C26" s="4">
-        <f>SUM(Q27:S27)</f>
-        <v>0</v>
+        <f>SUM(AA26:AH26)</f>
+        <v>2</v>
       </c>
       <c r="D26" s="5"/>
       <c r="P26" s="6"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U26" s="6"/>
+      <c r="V26" s="7"/>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="6"/>
+      <c r="AF26">
+        <v>1</v>
+      </c>
+      <c r="AG26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -1141,75 +1468,100 @@
       <c r="C27" s="1"/>
       <c r="D27" s="5"/>
       <c r="P27" s="6"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U27" s="6"/>
+      <c r="V27" s="7"/>
+      <c r="Z27" s="6"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="4">
-        <f>SUM(D28:P28)</f>
-        <v>0</v>
+        <f>SUM(D28:Z28)</f>
+        <v>5</v>
       </c>
       <c r="C28" s="4">
-        <f>SUM(Q29:S29)</f>
-        <v>0</v>
+        <f>SUM(AA28:AH28)</f>
+        <v>2</v>
       </c>
       <c r="D28" s="5"/>
       <c r="P28" s="6"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U28" s="6"/>
+      <c r="V28" s="7">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28">
+        <v>1</v>
+      </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF28">
+        <v>1</v>
+      </c>
+      <c r="AG28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B31" s="4">
-        <f>SUM(D31:P31)</f>
+        <f>SUM(D31:Z31)</f>
         <v>1</v>
       </c>
       <c r="C31" s="4">
-        <f>SUM(Q32:S32)</f>
+        <f>SUM(AA31:AH31)</f>
         <v>1</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
-      <c r="R31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="AB31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="4">
-        <f>SUM(D32:P32)</f>
+        <f>SUM(D32:Z32)</f>
         <v>0</v>
       </c>
       <c r="C32" s="4">
-        <f>SUM(Q33:S33)</f>
-        <v>1</v>
-      </c>
-      <c r="R32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+        <f>SUM(AA32:AH32)</f>
+        <v>1</v>
+      </c>
+      <c r="AB32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="4">
-        <f>SUM(D33:P33)</f>
-        <v>3</v>
+        <f>SUM(D33:Z33)</f>
+        <v>4</v>
       </c>
       <c r="C33" s="4">
-        <f>SUM(Q34:S34)</f>
-        <v>0</v>
+        <f>SUM(AA33:AH33)</f>
+        <v>2</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -1220,41 +1572,47 @@
       <c r="J33">
         <v>1</v>
       </c>
-      <c r="S33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="AC33">
+        <v>1</v>
+      </c>
+      <c r="AD33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="4">
-        <f>SUM(D35:P35)</f>
+        <f>SUM(D35:Z35)</f>
         <v>0</v>
       </c>
       <c r="C35" s="4">
-        <f>SUM(Q36:S36)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+        <f>SUM(AA35:AH35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B36" s="4">
-        <f>SUM(D36:P36)</f>
-        <v>2</v>
+        <f>SUM(D36:Z36)</f>
+        <v>3</v>
       </c>
       <c r="C36" s="4">
-        <f>SUM(Q37:S37)</f>
-        <v>0</v>
+        <f>SUM(AA36:AH36)</f>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1262,28 +1620,31 @@
       <c r="E36">
         <v>1</v>
       </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q36" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="4">
-        <f>SUM(D38:P38)</f>
-        <v>2</v>
+        <f>SUM(D38:Z38)</f>
+        <v>6</v>
       </c>
       <c r="C38" s="4">
-        <f>SUM(Q39:S39)</f>
-        <v>1</v>
+        <f>SUM(AA38:AH38)</f>
+        <v>2</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1291,43 +1652,63 @@
       <c r="G38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q38" s="7">
+        <v>1</v>
+      </c>
+      <c r="R38" s="7">
+        <v>1</v>
+      </c>
+      <c r="S38" s="7">
+        <v>1</v>
+      </c>
+      <c r="T38" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD38">
+        <v>1</v>
+      </c>
+      <c r="AE38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="4">
-        <f>SUM(D39:P39)</f>
+        <f>SUM(D39:Z39)</f>
         <v>0</v>
       </c>
       <c r="C39" s="4">
-        <f>SUM(Q40:S40)</f>
-        <v>0</v>
-      </c>
-      <c r="R39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+        <f>SUM(AA39:AH39)</f>
+        <v>1</v>
+      </c>
+      <c r="AB39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B40" s="4">
-        <f>SUM(D40:P40)</f>
+        <f>SUM(D40:Z40)</f>
         <v>0</v>
       </c>
       <c r="C40" s="4">
-        <f>SUM(Q41:S41)</f>
+        <f>SUM(AA40:AH40)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D1:K1"/>
+    <mergeCell ref="Q1:U1"/>
     <mergeCell ref="L1:P1"/>
+    <mergeCell ref="V1:Z1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:C6 B8:C9 B11:C13 B17:C20 B22:C26 B28:C28 B31:C33 B35:C36 B38:C40">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="B17:C20 B22:C26 B28:C28 B31:C33 B35:C36 B38:C40 B4:C6 B8:C9 B11:C13">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>